<commit_message>
Storage added, show provinces
</commit_message>
<xml_diff>
--- a/storage/users.xlsx
+++ b/storage/users.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rafa\laravel\wd_game\storage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EA3BE00-E740-4334-8A9B-558E8E33D31E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{848BBBA0-49E7-4726-93F3-536C9B368A98}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11160" xr2:uid="{D612E0FD-AD0F-4EF5-B181-7127B4B121B4}"/>
   </bookViews>
@@ -31,13 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
-  <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>Prussia</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>Império Russo</t>
   </si>
@@ -45,16 +39,88 @@
     <t>França</t>
   </si>
   <si>
-    <t>img_slug</t>
-  </si>
-  <si>
-    <t>prussia.png</t>
-  </si>
-  <si>
-    <t>imperio_russo.png</t>
-  </si>
-  <si>
-    <t>franca.png</t>
+    <t>Espanha</t>
+  </si>
+  <si>
+    <t>Portugal</t>
+  </si>
+  <si>
+    <t>Bélgica</t>
+  </si>
+  <si>
+    <t>Países Baixos</t>
+  </si>
+  <si>
+    <t>Dinamarca</t>
+  </si>
+  <si>
+    <t>Reino Sueco</t>
+  </si>
+  <si>
+    <t>Baviera</t>
+  </si>
+  <si>
+    <t>Ducado de Baden</t>
+  </si>
+  <si>
+    <t>Áustria</t>
+  </si>
+  <si>
+    <t>Suíça</t>
+  </si>
+  <si>
+    <t>Sardenha-Piemonte</t>
+  </si>
+  <si>
+    <t>Parma</t>
+  </si>
+  <si>
+    <t>Lucca</t>
+  </si>
+  <si>
+    <t>Modena</t>
+  </si>
+  <si>
+    <t>Tuscany</t>
+  </si>
+  <si>
+    <t>Estados Papais</t>
+  </si>
+  <si>
+    <t>Duas Sicílias</t>
+  </si>
+  <si>
+    <t>Sérvia</t>
+  </si>
+  <si>
+    <t>Montenegro</t>
+  </si>
+  <si>
+    <t>Império Otomano</t>
+  </si>
+  <si>
+    <t>Moldávia</t>
+  </si>
+  <si>
+    <t>Valáquia</t>
+  </si>
+  <si>
+    <t>Grécia</t>
+  </si>
+  <si>
+    <t>Ilhas Jónicas</t>
+  </si>
+  <si>
+    <t>Reino Unido</t>
+  </si>
+  <si>
+    <t>Países Germânicos do Norte (não selecionáveis)</t>
+  </si>
+  <si>
+    <t>Württemberg</t>
+  </si>
+  <si>
+    <t>Prússia</t>
   </si>
 </sst>
 </file>
@@ -105,15 +171,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -429,56 +489,174 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AC02550-6D23-420B-B912-BE8567ED8E04}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="A4" sqref="A4:A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="19.5703125" customWidth="1"/>
     <col min="3" max="3" width="17" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" s="1"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="B3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" t="s">
-        <v>7</v>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="rafa@ribe" xr:uid="{A293AA0B-A9FB-4FC1-8737-8AEFCBD4B54C}"/>
-    <hyperlink ref="B3" r:id="rId2" display="davi@davi" xr:uid="{CEAFB40A-6851-416B-BDFD-D18A6B135293}"/>
+    <hyperlink ref="A1" r:id="rId1" display="rafa@ribe" xr:uid="{78DE9457-A90F-4C75-ADA5-0F02D36F1C39}"/>
+    <hyperlink ref="A2" r:id="rId2" display="davi@davi" xr:uid="{98326220-BDA7-4699-A513-664DD0B8F680}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>

</xml_diff>